<commit_message>
Commit một số demo có thể tham khảo cho các chức năng. Cập nhật cột tham khảo cho GameFeatureChecklist.xlsx
</commit_message>
<xml_diff>
--- a/GameFeatureChecklist.xlsx
+++ b/GameFeatureChecklist.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
   <si>
     <t>STT</t>
   </si>
@@ -161,12 +161,36 @@
 - Dùng resource giống bản preview (không khuyến khích - cái này của C4W nên có thể trùng với nhóm khác) hoặc resource đính kèm hoặc resource khác trên mạng.</t>
     </r>
   </si>
+  <si>
+    <t>Tham khảo</t>
+  </si>
+  <si>
+    <t>State1.txt</t>
+  </si>
+  <si>
+    <t>Môn XML</t>
+  </si>
+  <si>
+    <t>Phần hiển thị menu chính</t>
+  </si>
+  <si>
+    <t>8.NotSoHealthy</t>
+  </si>
+  <si>
+    <t>2.WalkingSpriteDemo</t>
+  </si>
+  <si>
+    <t>3.JumpingSpriteDemo</t>
+  </si>
+  <si>
+    <t>5.thewizardshooting</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -227,6 +251,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="7" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -236,7 +267,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -259,11 +290,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -316,8 +384,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -613,7 +689,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:C1"/>
@@ -624,26 +700,30 @@
     <col min="1" max="1" width="4" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" customWidth="1"/>
-    <col min="4" max="4" width="99.85546875" customWidth="1"/>
-    <col min="5" max="5" width="5.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="85.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="6" width="5.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" s="17" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="17"/>
-      <c r="D1" s="18">
+      <c r="D1" s="21">
         <v>40665</v>
       </c>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="18">
+        <v>40721</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="15" t="s">
         <v>0</v>
       </c>
@@ -656,17 +736,20 @@
       <c r="D2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="G2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="H2" s="8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="195">
+    <row r="3" spans="1:8" ht="210">
       <c r="A3" s="16">
         <v>1</v>
       </c>
@@ -679,16 +762,19 @@
       <c r="D3" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="11"/>
-      <c r="F3" s="12" t="s">
+      <c r="E3" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="11"/>
+      <c r="G3" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="14">
+      <c r="H3" s="14">
         <f>$D$1+21</f>
         <v>40686</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8">
       <c r="A4" s="16">
         <v>2</v>
       </c>
@@ -701,16 +787,19 @@
       <c r="D4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="11"/>
-      <c r="F4" s="12" t="s">
+      <c r="E4" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="11"/>
+      <c r="G4" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="14">
+      <c r="H4" s="14">
         <f>$D$1+21</f>
         <v>40686</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:8">
       <c r="A5" s="16">
         <v>3</v>
       </c>
@@ -723,11 +812,14 @@
       <c r="D5" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="11"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="13"/>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="E5" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" s="11"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="13"/>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="16">
         <v>4</v>
       </c>
@@ -740,11 +832,14 @@
       <c r="D6" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="13"/>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="E6" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="11"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="13"/>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="16">
         <v>5</v>
       </c>
@@ -757,11 +852,12 @@
       <c r="D7" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="11"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="13"/>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="E7" s="19"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="13"/>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="16">
         <v>6</v>
       </c>
@@ -774,11 +870,12 @@
       <c r="D8" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="11"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="13"/>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="E8" s="19"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="13"/>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="16">
         <v>7</v>
       </c>
@@ -789,11 +886,14 @@
       <c r="D9" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="11"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="13"/>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="E9" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" s="11"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="13"/>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="16">
         <v>8</v>
       </c>
@@ -804,11 +904,12 @@
       <c r="D10" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="11"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="13"/>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="E10" s="19"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="13"/>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="16">
         <v>9</v>
       </c>
@@ -819,11 +920,14 @@
       <c r="D11" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="E11" s="11"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="13"/>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="E11" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="11"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="13"/>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" s="16">
         <v>10</v>
       </c>
@@ -834,11 +938,14 @@
       <c r="D12" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="11"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="13"/>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="E12" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="11"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="13"/>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" s="16">
         <v>11</v>
       </c>
@@ -851,16 +958,17 @@
       <c r="D13" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="11"/>
-      <c r="F13" s="12" t="s">
+      <c r="E13" s="19"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="G13" s="14">
+      <c r="H13" s="14">
         <f>$D$1+21</f>
         <v>40686</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:8">
       <c r="A14" s="16">
         <v>12</v>
       </c>
@@ -873,20 +981,22 @@
       <c r="D14" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="11"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="13"/>
-    </row>
-    <row r="15" spans="1:7">
+      <c r="E14" s="19"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="13"/>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" s="16">
         <v>13</v>
       </c>
       <c r="B15" s="16"/>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="13"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Xây dựng hoàn chỉnh lớp MySong.cs Bổ sung các file sound effect (wav). Cải tiến việc chọn Menu.cs Chỉnh sửa vị trí hiển thị nhân vật. Tổ chức lại cấu trúc thư mục.
</commit_message>
<xml_diff>
--- a/GameFeatureChecklist.xlsx
+++ b/GameFeatureChecklist.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>STT</t>
   </si>
@@ -162,9 +162,6 @@
     <t>Tham khảo</t>
   </si>
   <si>
-    <t>State1.txt</t>
-  </si>
-  <si>
     <t>Môn XML</t>
   </si>
   <si>
@@ -181,6 +178,15 @@
   </si>
   <si>
     <t>5.thewizardshooting</t>
+  </si>
+  <si>
+    <t>Các tập tin màn chơi của môn C4W</t>
+  </si>
+  <si>
+    <t>Demo</t>
+  </si>
+  <si>
+    <t>Quay phim demo chương trình, có tiếng, định dạng nhẹ</t>
   </si>
 </sst>
 </file>
@@ -371,8 +377,30 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -381,24 +409,6 @@
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -707,24 +717,24 @@
     <col min="2" max="2" width="3.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" customWidth="1"/>
     <col min="4" max="4" width="85.7109375" customWidth="1"/>
-    <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="5.5703125" style="22" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.5703125" style="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" style="19" customWidth="1"/>
+    <col min="6" max="6" width="5.5703125" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" style="14" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="15">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="21">
         <v>40665</v>
       </c>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
       <c r="H1" s="11">
         <v>40721</v>
       </c>
@@ -742,13 +752,13 @@
       <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="17" t="s">
+      <c r="G2" s="12" t="s">
         <v>4</v>
       </c>
       <c r="H2" s="4" t="s">
@@ -768,11 +778,11 @@
       <c r="D3" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E3" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="F3" s="21"/>
-      <c r="G3" s="18">
+      <c r="E3" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" s="16"/>
+      <c r="G3" s="13">
         <v>1</v>
       </c>
       <c r="H3" s="8">
@@ -793,16 +803,15 @@
       <c r="D4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="F4" s="21"/>
-      <c r="G4" s="18">
-        <v>1</v>
+      <c r="E4" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="16"/>
+      <c r="G4" s="13">
+        <v>0.5</v>
       </c>
       <c r="H4" s="8">
-        <f>$D$1+21</f>
-        <v>40686</v>
+        <v>40719</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -818,15 +827,13 @@
       <c r="D5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="F5" s="21">
+      <c r="E5" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="16">
         <v>1</v>
       </c>
-      <c r="G5" s="18">
-        <v>0.5</v>
-      </c>
+      <c r="G5" s="13"/>
       <c r="H5" s="7"/>
     </row>
     <row r="6" spans="1:8">
@@ -842,13 +849,13 @@
       <c r="D6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="F6" s="21">
+      <c r="E6" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="16">
         <v>0</v>
       </c>
-      <c r="G6" s="18"/>
+      <c r="G6" s="13"/>
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:8">
@@ -864,11 +871,11 @@
       <c r="D7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="12"/>
-      <c r="F7" s="21">
+      <c r="E7" s="5"/>
+      <c r="F7" s="16">
         <v>0</v>
       </c>
-      <c r="G7" s="18"/>
+      <c r="G7" s="13"/>
       <c r="H7" s="7"/>
     </row>
     <row r="8" spans="1:8">
@@ -884,11 +891,11 @@
       <c r="D8" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="12"/>
-      <c r="F8" s="21">
+      <c r="E8" s="5"/>
+      <c r="F8" s="16">
         <v>0</v>
       </c>
-      <c r="G8" s="18"/>
+      <c r="G8" s="13"/>
       <c r="H8" s="7"/>
     </row>
     <row r="9" spans="1:8">
@@ -902,13 +909,13 @@
       <c r="D9" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="F9" s="21">
+      <c r="E9" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="16">
         <v>0</v>
       </c>
-      <c r="G9" s="18"/>
+      <c r="G9" s="13"/>
       <c r="H9" s="7"/>
     </row>
     <row r="10" spans="1:8">
@@ -922,11 +929,11 @@
       <c r="D10" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="12"/>
-      <c r="F10" s="21">
+      <c r="E10" s="5"/>
+      <c r="F10" s="16">
         <v>0</v>
       </c>
-      <c r="G10" s="18"/>
+      <c r="G10" s="13"/>
       <c r="H10" s="7"/>
     </row>
     <row r="11" spans="1:8">
@@ -940,13 +947,13 @@
       <c r="D11" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="F11" s="21">
+      <c r="E11" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="16">
         <v>0</v>
       </c>
-      <c r="G11" s="18"/>
+      <c r="G11" s="13"/>
       <c r="H11" s="7"/>
     </row>
     <row r="12" spans="1:8">
@@ -960,13 +967,13 @@
       <c r="D12" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E12" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="F12" s="21">
+      <c r="E12" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" s="16">
         <v>0</v>
       </c>
-      <c r="G12" s="18"/>
+      <c r="G12" s="13"/>
       <c r="H12" s="7"/>
     </row>
     <row r="13" spans="1:8">
@@ -982,9 +989,9 @@
       <c r="D13" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="12"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="18">
+      <c r="E13" s="5"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="13">
         <v>1</v>
       </c>
       <c r="H13" s="8">
@@ -1005,24 +1012,34 @@
       <c r="D14" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="12"/>
-      <c r="F14" s="21">
-        <v>0.1</v>
-      </c>
-      <c r="G14" s="18"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="16">
+        <v>1</v>
+      </c>
+      <c r="G14" s="13"/>
       <c r="H14" s="7"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="10">
         <v>13</v>
       </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="7"/>
+      <c r="B15" s="10">
+        <v>7</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="5"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="13">
+        <v>0</v>
+      </c>
+      <c r="H15" s="8">
+        <v>40721</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Cải tiến collision detection (có thể ăn đồng tiền). Sửa sprite Run, bỏ Running. Sửa map (logic hơn, nhiều quái vật hơn). Thêm thanh HP và số lượng Coin. Thông báo về quay phim demo (trong Noi dung can nop.txt).
</commit_message>
<xml_diff>
--- a/GameFeatureChecklist.xlsx
+++ b/GameFeatureChecklist.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>STT</t>
   </si>
@@ -181,12 +181,6 @@
   </si>
   <si>
     <t>Các tập tin màn chơi của môn C4W</t>
-  </si>
-  <si>
-    <t>Demo</t>
-  </si>
-  <si>
-    <t>Quay phim demo chương trình, có tiếng, định dạng nhẹ</t>
   </si>
 </sst>
 </file>
@@ -705,7 +699,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:C1"/>
@@ -831,7 +825,7 @@
         <v>39</v>
       </c>
       <c r="F5" s="16">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="G5" s="13"/>
       <c r="H5" s="7"/>
@@ -853,7 +847,7 @@
         <v>40</v>
       </c>
       <c r="F6" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" s="13"/>
       <c r="H6" s="7"/>
@@ -873,7 +867,7 @@
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="16">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="G7" s="13"/>
       <c r="H7" s="7"/>
@@ -951,7 +945,7 @@
         <v>41</v>
       </c>
       <c r="F11" s="16">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="G11" s="13"/>
       <c r="H11" s="7"/>
@@ -1018,28 +1012,6 @@
       </c>
       <c r="G14" s="13"/>
       <c r="H14" s="7"/>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="10">
-        <v>13</v>
-      </c>
-      <c r="B15" s="10">
-        <v>7</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="13">
-        <v>0</v>
-      </c>
-      <c r="H15" s="8">
-        <v>40721</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Cập nhật báo cáo và nội dung đã thực hiện.
</commit_message>
<xml_diff>
--- a/GameFeatureChecklist.xlsx
+++ b/GameFeatureChecklist.xlsx
@@ -925,7 +925,7 @@
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="16">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G10" s="13"/>
       <c r="H10" s="7"/>
@@ -945,7 +945,7 @@
         <v>41</v>
       </c>
       <c r="F11" s="16">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="G11" s="13"/>
       <c r="H11" s="7"/>
@@ -965,7 +965,7 @@
         <v>42</v>
       </c>
       <c r="F12" s="16">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="G12" s="13"/>
       <c r="H12" s="7"/>

</xml_diff>

<commit_message>
Xử lý nhảy, bắn cơ bản.
</commit_message>
<xml_diff>
--- a/GameFeatureChecklist.xlsx
+++ b/GameFeatureChecklist.xlsx
@@ -907,7 +907,7 @@
         <v>43</v>
       </c>
       <c r="F9" s="16">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="G9" s="13"/>
       <c r="H9" s="7"/>
@@ -945,7 +945,7 @@
         <v>41</v>
       </c>
       <c r="F11" s="16">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="G11" s="13"/>
       <c r="H11" s="7"/>
@@ -965,7 +965,7 @@
         <v>42</v>
       </c>
       <c r="F12" s="16">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="G12" s="13"/>
       <c r="H12" s="7"/>

</xml_diff>

<commit_message>
Xử lý tiếp nhảy (jump up, jump over) và bắn (shoot).
</commit_message>
<xml_diff>
--- a/GameFeatureChecklist.xlsx
+++ b/GameFeatureChecklist.xlsx
@@ -887,7 +887,7 @@
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="16">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G8" s="13"/>
       <c r="H8" s="7"/>
@@ -907,7 +907,7 @@
         <v>43</v>
       </c>
       <c r="F9" s="16">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="G9" s="13"/>
       <c r="H9" s="7"/>
@@ -945,7 +945,7 @@
         <v>41</v>
       </c>
       <c r="F11" s="16">
-        <v>0.6</v>
+        <v>0.75</v>
       </c>
       <c r="G11" s="13"/>
       <c r="H11" s="7"/>
@@ -965,7 +965,7 @@
         <v>42</v>
       </c>
       <c r="F12" s="16">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="G12" s="13"/>
       <c r="H12" s="7"/>

</xml_diff>

<commit_message>
Xử lý nhảy. Xử lý chắc năng game over khi hết HP.
</commit_message>
<xml_diff>
--- a/GameFeatureChecklist.xlsx
+++ b/GameFeatureChecklist.xlsx
@@ -702,7 +702,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -887,7 +887,7 @@
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="16">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="G8" s="13"/>
       <c r="H8" s="7"/>
@@ -965,7 +965,7 @@
         <v>42</v>
       </c>
       <c r="F12" s="16">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="G12" s="13"/>
       <c r="H12" s="7"/>

</xml_diff>